<commit_message>
circle movement + level logic full
</commit_message>
<xml_diff>
--- a/Angles_Circle.xlsx
+++ b/Angles_Circle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Gold_Miner_FPGA\game\RTL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nirko\Documents\Degree\Electrical_Eng_Lab_1\Gold_Miner_FPGA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53BC396F-4794-4FD3-AC96-C14987032A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1018D41F-0EEF-47D2-A296-DC13888A3531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{18540158-1936-4FDD-B369-05A21AAFCE80}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{18540158-1936-4FDD-B369-05A21AAFCE80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>alpha(deg)</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>1024*cos</t>
+  </si>
+  <si>
+    <t>round sin</t>
+  </si>
+  <si>
+    <t>round cos</t>
   </si>
 </sst>
 </file>
@@ -425,20 +431,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771AAE51-7FD4-415A-9361-D9BB4E37374E}">
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:I92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q93" sqref="Q93"/>
+      <selection activeCell="I2" sqref="I2:I92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.46484375" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,8 +463,14 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -482,8 +494,20 @@
         <f xml:space="preserve"> 1024*D2</f>
         <v>1024</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2">
+        <f>ROUND(E2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>ROUND(F2,0)</f>
+        <v>1024</v>
+      </c>
+      <c r="I2" t="str">
+        <f>_xlfn.CONCAT("{10'd",G2, ", 10'd",H2,"},")</f>
+        <v>{10'd0, 10'd1024},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3">
         <f xml:space="preserve"> A2 + 1</f>
         <v>1</v>
@@ -501,17 +525,29 @@
         <v>0.99984769515639127</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E66" si="3" xml:space="preserve"> 1024*C3</f>
+        <f t="shared" ref="E3:F66" si="3" xml:space="preserve"> 1024*C3</f>
         <v>17.871264191778316</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F66" si="4" xml:space="preserve"> 1024*D3</f>
+        <f t="shared" si="3"/>
         <v>1023.8440398401447</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3">
+        <f t="shared" ref="G3:H66" si="4">ROUND(E3,0)</f>
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="4"/>
+        <v>1024</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I66" si="5">_xlfn.CONCAT("{10'd",G3, ", 10'd",H3,"},")</f>
+        <v>{10'd18, 10'd1024},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4">
-        <f t="shared" ref="A4:A67" si="5" xml:space="preserve"> A3 + 1</f>
+        <f t="shared" ref="A4:A67" si="6" xml:space="preserve"> A3 + 1</f>
         <v>2</v>
       </c>
       <c r="B4">
@@ -531,13 +567,25 @@
         <v>35.737084623360992</v>
       </c>
       <c r="F4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1023.3762068675541</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="4"/>
+        <v>1023</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd36, 10'd1023},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="B5">
@@ -557,13 +605,25 @@
         <v>53.592019192774487</v>
       </c>
       <c r="F5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1022.5966435886836</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <f t="shared" si="4"/>
+        <v>54</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="4"/>
+        <v>1023</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd54, 10'd1023},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="B6">
@@ -583,13 +643,25 @@
         <v>71.43062911398431</v>
       </c>
       <c r="F6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1021.50558746606</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6">
+        <f t="shared" si="4"/>
+        <v>71</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="4"/>
+        <v>1022</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd71, 10'd1022},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="B7">
@@ -609,13 +681,25 @@
         <v>89.247480573601962</v>
       </c>
       <c r="F7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1020.1033708459474</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7">
+        <f t="shared" si="4"/>
+        <v>89</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="4"/>
+        <v>1020</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd89, 10'd1020},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="B8">
@@ -635,13 +719,25 @@
         <v>107.03714638607715</v>
       </c>
       <c r="F8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1018.3904208571118</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8">
+        <f t="shared" si="4"/>
+        <v>107</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="4"/>
+        <v>1018</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd107, 10'd1018},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="B9">
@@ -661,13 +757,25 @@
         <v>124.79420764687102</v>
       </c>
       <c r="F9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1016.3672592807137</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9">
+        <f t="shared" si="4"/>
+        <v>125</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="4"/>
+        <v>1016</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd125, 10'd1016},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="B10">
@@ -687,13 +795,25 @@
         <v>142.51325538310701</v>
       </c>
       <c r="F10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1014.0345023913681</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10">
+        <f t="shared" si="4"/>
+        <v>143</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="4"/>
+        <v>1014</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd143, 10'd1014},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="B11">
@@ -713,13 +833,25 @@
         <v>160.18889220119641</v>
       </c>
       <c r="F11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1011.3928607694211</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="4"/>
+        <v>1011</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd160, 10'd1011},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="B12">
@@ -739,13 +871,25 @@
         <v>177.81573393093666</v>
       </c>
       <c r="F12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1008.443139084501</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12">
+        <f t="shared" si="4"/>
+        <v>178</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="4"/>
+        <v>1008</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd178, 10'd1008},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="B13">
@@ -765,13 +909,25 @@
         <v>195.38841126558188</v>
       </c>
       <c r="F13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1005.1862358504079</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13">
+        <f t="shared" si="4"/>
+        <v>195</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="4"/>
+        <v>1005</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd195, 10'd1005},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="B14">
@@ -791,13 +947,25 @@
         <v>212.90157139738557</v>
       </c>
       <c r="F14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1001.623143151417</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14">
+        <f t="shared" si="4"/>
+        <v>213</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="4"/>
+        <v>1002</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd213, 10'd1002},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="B15">
@@ -817,13 +985,25 @@
         <v>230.34987964811776</v>
       </c>
       <c r="F15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>997.75494634008089</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15">
+        <f t="shared" si="4"/>
+        <v>230</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="4"/>
+        <v>998</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd230, 10'd998},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="B16">
@@ -843,13 +1023,25 @@
         <v>247.72802109405976</v>
       </c>
       <c r="F16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>993.58282370662039</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16">
+        <f t="shared" si="4"/>
+        <v>248</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
+        <v>994</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd248, 10'd994},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="B17">
@@ -869,13 +1061,25 @@
         <v>265.03070218498124</v>
       </c>
       <c r="F17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>989.10804612000595</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17">
+        <f t="shared" si="4"/>
+        <v>265</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="4"/>
+        <v>989</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd265, 10'd989},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="B18">
@@ -895,13 +1099,25 @@
         <v>282.25265235660714</v>
       </c>
       <c r="F18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>984.33197664083855</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18">
+        <f t="shared" si="4"/>
+        <v>282</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="4"/>
+        <v>984</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd282, 10'd984},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="B19">
@@ -921,13 +1137,25 @@
         <v>299.38862563608245</v>
       </c>
       <c r="F19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>979.25607010614829</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19">
+        <f t="shared" si="4"/>
+        <v>299</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="4"/>
+        <v>979</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd299, 10'd979},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="B20">
@@ -947,13 +1175,25 @@
         <v>316.43340223994613</v>
       </c>
       <c r="F20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>973.88187268623722</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20">
+        <f t="shared" si="4"/>
+        <v>316</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="4"/>
+        <v>974</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd316, 10'd974},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="B21">
@@ -973,13 +1213,25 @@
         <v>333.38179016412846</v>
       </c>
       <c r="F21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>968.21102141370045</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21">
+        <f t="shared" si="4"/>
+        <v>333</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="4"/>
+        <v>968</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd333, 10'd968},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="B22">
@@ -999,13 +1251,25 @@
         <v>350.22862676548476</v>
       </c>
       <c r="F22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>962.24524368477023</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22">
+        <f t="shared" si="4"/>
+        <v>350</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="4"/>
+        <v>962</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd350, 10'd962},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="B23">
@@ -1025,13 +1289,25 @@
         <v>366.96878033438747</v>
       </c>
       <c r="F23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>955.98635673313458</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23">
+        <f t="shared" si="4"/>
+        <v>367</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="4"/>
+        <v>956</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd367, 10'd956},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="B24">
@@ -1051,13 +1327,25 @@
         <v>383.5971516578939</v>
       </c>
       <c r="F24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>949.43626707639032</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24">
+        <f t="shared" si="4"/>
+        <v>384</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="4"/>
+        <v>949</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd384, 10'd949},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
       <c r="B25">
@@ -1077,13 +1365,25 @@
         <v>400.10867557301634</v>
       </c>
       <c r="F25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>942.59696993529894</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25">
+        <f t="shared" si="4"/>
+        <v>400</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="4"/>
+        <v>943</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd400, 10'd943},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="B26">
@@ -1103,13 +1403,25 @@
         <v>416.49832250961941</v>
       </c>
       <c r="F26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>935.47054862602329</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26">
+        <f t="shared" si="4"/>
+        <v>416</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="4"/>
+        <v>935</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd416, 10'd935},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="B27">
@@ -1129,13 +1441,25 @@
         <v>432.76110002247623</v>
       </c>
       <c r="F27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>928.05917392552954</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27">
+        <f t="shared" si="4"/>
+        <v>433</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="4"/>
+        <v>928</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd433, 10'd928},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>26</v>
       </c>
       <c r="B28">
@@ -1155,13 +1479,25 @@
         <v>448.89205431201526</v>
       </c>
       <c r="F28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>920.36510341034705</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28">
+        <f t="shared" si="4"/>
+        <v>449</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="4"/>
+        <v>920</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd449, 10'd920},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="B29">
@@ -1181,13 +1517,25 @@
         <v>464.88627173329587</v>
       </c>
       <c r="F29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>912.39068076888873</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G29">
+        <f t="shared" si="4"/>
+        <v>465</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="4"/>
+        <v>912</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd465, 10'd912},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
       <c r="B30">
@@ -1207,13 +1555,25 @@
         <v>480.73888029275219</v>
       </c>
       <c r="F30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>904.13833508754124</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G30">
+        <f t="shared" si="4"/>
+        <v>481</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="4"/>
+        <v>904</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd481, 10'd904},</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>29</v>
       </c>
       <c r="B31">
@@ -1233,13 +1593,25 @@
         <v>496.44505113224915</v>
       </c>
       <c r="F31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>895.61058011074124</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G31">
+        <f t="shared" si="4"/>
+        <v>496</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="4"/>
+        <v>896</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd496, 10'd896},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="B32">
@@ -1259,13 +1631,25 @@
         <v>511.99999999999994</v>
       </c>
       <c r="F32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>886.81001347526524</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G32">
+        <f t="shared" si="4"/>
+        <v>512</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="4"/>
+        <v>887</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd512, 10'd887},</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>31</v>
       </c>
       <c r="B33">
@@ -1285,13 +1669,25 @@
         <v>527.39898870789546</v>
       </c>
       <c r="F33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>877.73931591896303</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G33">
+        <f t="shared" si="4"/>
+        <v>527</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="4"/>
+        <v>878</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd527, 10'd878},</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="B34">
@@ -1311,13 +1707,25 @@
         <v>542.63732657480182</v>
       </c>
       <c r="F34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>868.40125046418018</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G34">
+        <f t="shared" si="4"/>
+        <v>543</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="4"/>
+        <v>868</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd543, 10'd868},</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>33</v>
       </c>
       <c r="B35">
@@ -1337,13 +1745,25 @@
         <v>557.71037185538773</v>
       </c>
       <c r="F35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>858.79866157611423</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G35">
+        <f t="shared" si="4"/>
+        <v>558</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="4"/>
+        <v>859</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd558, 10'd859},</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>34</v>
       </c>
       <c r="B36">
@@ -1363,13 +1783,25 @@
         <v>572.61353315404483</v>
       </c>
       <c r="F36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>848.93447429636262</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G36">
+        <f t="shared" si="4"/>
+        <v>573</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="4"/>
+        <v>849</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd573, 10'd849},</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>35</v>
       </c>
       <c r="B37">
@@ -1389,13 +1821,25 @@
         <v>587.34227082347115</v>
       </c>
       <c r="F37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>838.8116933519276</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G37">
+        <f t="shared" si="4"/>
+        <v>587</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="4"/>
+        <v>839</v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd587, 10'd839},</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>36</v>
       </c>
       <c r="B38">
@@ -1415,13 +1859,25 @@
         <v>601.89209834749249</v>
       </c>
       <c r="F38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>828.43340223994619</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G38">
+        <f t="shared" si="4"/>
+        <v>602</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="4"/>
+        <v>828</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd602, 10'd828},</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="B39">
@@ -1441,13 +1897,25 @@
         <v>616.25858370769743</v>
       </c>
       <c r="F39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>817.80276228842786</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G39">
+        <f t="shared" si="4"/>
+        <v>616</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="4"/>
+        <v>818</v>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd616, 10'd818},</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>38</v>
       </c>
       <c r="B40">
@@ -1467,13 +1935,25 @@
         <v>630.43735073347409</v>
       </c>
       <c r="F40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>806.92301169328323</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G40">
+        <f t="shared" si="4"/>
+        <v>630</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="4"/>
+        <v>807</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd630, 10'd807},</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>39</v>
       </c>
       <c r="B41">
@@ -1493,13 +1973,25 @@
         <v>644.42408043503349</v>
       </c>
       <c r="F41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>795.7974645319382</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G41">
+        <f t="shared" si="4"/>
+        <v>644</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="4"/>
+        <v>796</v>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd644, 10'd796},</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="B42">
@@ -1519,13 +2011,25 @@
         <v>658.21451231901619</v>
       </c>
       <c r="F42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>784.42950975383349</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G42">
+        <f t="shared" si="4"/>
+        <v>658</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="4"/>
+        <v>784</v>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd658, 10'd784},</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>41</v>
       </c>
       <c r="B43">
@@ -1545,13 +2049,25 @@
         <v>671.80444568627945</v>
       </c>
       <c r="F43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>772.82261014811854</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G43">
+        <f t="shared" si="4"/>
+        <v>672</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="4"/>
+        <v>773</v>
+      </c>
+      <c r="I43" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd672, 10'd773},</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>42</v>
       </c>
       <c r="B44">
@@ -1571,13 +2087,25 @@
         <v>685.18974091147084</v>
       </c>
       <c r="F44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>760.98030128885171</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G44">
+        <f t="shared" si="4"/>
+        <v>685</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="4"/>
+        <v>761</v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd685, 10'd761},</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43</v>
       </c>
       <c r="B45">
@@ -1597,13 +2125,25 @@
         <v>698.36632070399844</v>
       </c>
       <c r="F45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>748.90619045803055</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G45">
+        <f t="shared" si="4"/>
+        <v>698</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="4"/>
+        <v>749</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd698, 10'd749},</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44</v>
       </c>
       <c r="B46">
@@ -1623,13 +2163,25 @@
         <v>711.33017135001319</v>
       </c>
       <c r="F46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>736.60395554677882</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G46">
+        <f t="shared" si="4"/>
+        <v>711</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="4"/>
+        <v>737</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd711, 10'd737},</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>45</v>
       </c>
       <c r="B47">
@@ -1649,13 +2201,25 @@
         <v>724.0773439350246</v>
       </c>
       <c r="F47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>724.07734393502471</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G47">
+        <f t="shared" si="4"/>
+        <v>724</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="4"/>
+        <v>724</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd724, 10'd724},</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>46</v>
       </c>
       <c r="B48">
@@ -1675,13 +2239,25 @@
         <v>736.60395554677871</v>
       </c>
       <c r="F48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>711.33017135001319</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G48">
+        <f t="shared" si="4"/>
+        <v>737</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="4"/>
+        <v>711</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd737, 10'd711},</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>47</v>
       </c>
       <c r="B49">
@@ -1701,13 +2277,25 @@
         <v>748.90619045803055</v>
       </c>
       <c r="F49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>698.36632070399844</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G49">
+        <f t="shared" si="4"/>
+        <v>749</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="4"/>
+        <v>698</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd749, 10'd698},</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
       <c r="B50">
@@ -1727,13 +2315,25 @@
         <v>760.98030128885171</v>
       </c>
       <c r="F50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>685.18974091147084</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G50">
+        <f t="shared" si="4"/>
+        <v>761</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="4"/>
+        <v>685</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd761, 10'd685},</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>49</v>
       </c>
       <c r="B51">
@@ -1753,13 +2353,25 @@
         <v>772.82261014811854</v>
       </c>
       <c r="F51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>671.80444568627945</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G51">
+        <f t="shared" si="4"/>
+        <v>773</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="4"/>
+        <v>672</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd773, 10'd672},</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="B52">
@@ -1779,13 +2391,25 @@
         <v>784.42950975383349</v>
       </c>
       <c r="F52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>658.21451231901631</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G52">
+        <f t="shared" si="4"/>
+        <v>784</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="4"/>
+        <v>658</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd784, 10'd658},</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>51</v>
       </c>
       <c r="B53">
@@ -1805,13 +2429,25 @@
         <v>795.7974645319382</v>
       </c>
       <c r="F53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>644.4240804350336</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G53">
+        <f t="shared" si="4"/>
+        <v>796</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="4"/>
+        <v>644</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd796, 10'd644},</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>52</v>
       </c>
       <c r="B54">
@@ -1831,13 +2467,25 @@
         <v>806.92301169328334</v>
       </c>
       <c r="F54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>630.43735073347409</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G54">
+        <f t="shared" si="4"/>
+        <v>807</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="4"/>
+        <v>630</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd807, 10'd630},</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>53</v>
       </c>
       <c r="B55">
@@ -1857,13 +2505,25 @@
         <v>817.80276228842786</v>
       </c>
       <c r="F55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>616.25858370769754</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G55">
+        <f t="shared" si="4"/>
+        <v>818</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="4"/>
+        <v>616</v>
+      </c>
+      <c r="I55" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd818, 10'd616},</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>54</v>
       </c>
       <c r="B56">
@@ -1883,13 +2543,25 @@
         <v>828.43340223994619</v>
       </c>
       <c r="F56">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>601.89209834749249</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G56">
+        <f t="shared" si="4"/>
+        <v>828</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="4"/>
+        <v>602</v>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd828, 10'd602},</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="B57">
@@ -1909,13 +2581,25 @@
         <v>838.8116933519276</v>
       </c>
       <c r="F57">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>587.34227082347127</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G57">
+        <f t="shared" si="4"/>
+        <v>839</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="4"/>
+        <v>587</v>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd839, 10'd587},</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>56</v>
       </c>
       <c r="B58">
@@ -1935,13 +2619,25 @@
         <v>848.93447429636274</v>
       </c>
       <c r="F58">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>572.61353315404472</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G58">
+        <f t="shared" si="4"/>
+        <v>849</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="4"/>
+        <v>573</v>
+      </c>
+      <c r="I58" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd849, 10'd573},</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
       <c r="B59">
@@ -1961,13 +2657,25 @@
         <v>858.79866157611423</v>
       </c>
       <c r="F59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>557.71037185538773</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G59">
+        <f t="shared" si="4"/>
+        <v>859</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="4"/>
+        <v>558</v>
+      </c>
+      <c r="I59" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd859, 10'd558},</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>58</v>
       </c>
       <c r="B60">
@@ -1987,13 +2695,25 @@
         <v>868.40125046418018</v>
       </c>
       <c r="F60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>542.63732657480182</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G60">
+        <f t="shared" si="4"/>
+        <v>868</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="4"/>
+        <v>543</v>
+      </c>
+      <c r="I60" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd868, 10'd543},</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>59</v>
       </c>
       <c r="B61">
@@ -2013,13 +2733,25 @@
         <v>877.73931591896303</v>
       </c>
       <c r="F61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>527.39898870789546</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G61">
+        <f t="shared" si="4"/>
+        <v>878</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="4"/>
+        <v>527</v>
+      </c>
+      <c r="I61" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd878, 10'd527},</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="B62">
@@ -2039,13 +2771,25 @@
         <v>886.81001347526512</v>
       </c>
       <c r="F62">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>512.00000000000011</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G62">
+        <f t="shared" si="4"/>
+        <v>887</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="4"/>
+        <v>512</v>
+      </c>
+      <c r="I62" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd887, 10'd512},</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>61</v>
       </c>
       <c r="B63">
@@ -2065,13 +2809,25 @@
         <v>895.61058011074124</v>
       </c>
       <c r="F63">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>496.4450511322492</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G63">
+        <f t="shared" si="4"/>
+        <v>896</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="4"/>
+        <v>496</v>
+      </c>
+      <c r="I63" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd896, 10'd496},</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>62</v>
       </c>
       <c r="B64">
@@ -2091,13 +2847,25 @@
         <v>904.13833508754112</v>
       </c>
       <c r="F64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>480.73888029275224</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G64">
+        <f t="shared" si="4"/>
+        <v>904</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="4"/>
+        <v>481</v>
+      </c>
+      <c r="I64" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd904, 10'd481},</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>63</v>
       </c>
       <c r="B65">
@@ -2117,13 +2885,25 @@
         <v>912.39068076888861</v>
       </c>
       <c r="F65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>464.88627173329593</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G65">
+        <f t="shared" si="4"/>
+        <v>912</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="4"/>
+        <v>465</v>
+      </c>
+      <c r="I65" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd912, 10'd465},</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>64</v>
       </c>
       <c r="B66">
@@ -2143,684 +2923,1008 @@
         <v>920.36510341034705</v>
       </c>
       <c r="F66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>448.89205431201532</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G66">
+        <f t="shared" si="4"/>
+        <v>920</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="4"/>
+        <v>449</v>
+      </c>
+      <c r="I66" t="str">
+        <f t="shared" si="5"/>
+        <v>{10'd920, 10'd449},</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>65</v>
       </c>
       <c r="B67">
-        <f t="shared" ref="B67:B92" si="6">RADIANS(A67)</f>
+        <f t="shared" ref="B67:B92" si="7">RADIANS(A67)</f>
         <v>1.1344640137963142</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:C92" si="7" xml:space="preserve">  SIN(RADIANS(A67))</f>
+        <f t="shared" ref="C67:C92" si="8" xml:space="preserve">  SIN(RADIANS(A67))</f>
         <v>0.90630778703664994</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:D92" si="8" xml:space="preserve"> COS(RADIANS(A67))</f>
+        <f t="shared" ref="D67:D92" si="9" xml:space="preserve"> COS(RADIANS(A67))</f>
         <v>0.42261826174069944</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E92" si="9" xml:space="preserve"> 1024*C67</f>
+        <f t="shared" ref="E67:F92" si="10" xml:space="preserve"> 1024*C67</f>
         <v>928.05917392552954</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F92" si="10" xml:space="preserve"> 1024*D67</f>
+        <f t="shared" si="10"/>
         <v>432.76110002247623</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G67">
+        <f t="shared" ref="G67:H92" si="11">ROUND(E67,0)</f>
+        <v>928</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="11"/>
+        <v>433</v>
+      </c>
+      <c r="I67" t="str">
+        <f t="shared" ref="I67:I92" si="12">_xlfn.CONCAT("{10'd",G67, ", 10'd",H67,"},")</f>
+        <v>{10'd928, 10'd433},</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68">
-        <f t="shared" ref="A68:A90" si="11" xml:space="preserve"> A67 + 1</f>
+        <f t="shared" ref="A68:A90" si="13" xml:space="preserve"> A67 + 1</f>
         <v>66</v>
       </c>
       <c r="B68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1519173063162575</v>
       </c>
       <c r="C68">
+        <f t="shared" si="8"/>
+        <v>0.91354545764260087</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="9"/>
+        <v>0.40673664307580021</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="10"/>
+        <v>935.47054862602329</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="10"/>
+        <v>416.49832250961941</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="11"/>
+        <v>935</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="11"/>
+        <v>416</v>
+      </c>
+      <c r="I68" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd935, 10'd416},</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A69">
+        <f t="shared" si="13"/>
+        <v>67</v>
+      </c>
+      <c r="B69">
         <f t="shared" si="7"/>
-        <v>0.91354545764260087</v>
-      </c>
-      <c r="D68">
+        <v>1.1693705988362009</v>
+      </c>
+      <c r="C69">
         <f t="shared" si="8"/>
-        <v>0.40673664307580021</v>
-      </c>
-      <c r="E68">
+        <v>0.92050485345244037</v>
+      </c>
+      <c r="D69">
         <f t="shared" si="9"/>
-        <v>935.47054862602329</v>
-      </c>
-      <c r="F68">
-        <f t="shared" si="10"/>
-        <v>416.49832250961941</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69">
-        <f t="shared" si="11"/>
-        <v>67</v>
-      </c>
-      <c r="B69">
-        <f t="shared" si="6"/>
-        <v>1.1693705988362009</v>
-      </c>
-      <c r="C69">
+        <v>0.39073112848927372</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="10"/>
+        <v>942.59696993529894</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="10"/>
+        <v>400.10867557301628</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="11"/>
+        <v>943</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="11"/>
+        <v>400</v>
+      </c>
+      <c r="I69" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd943, 10'd400},</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A70">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="B70">
         <f t="shared" si="7"/>
-        <v>0.92050485345244037</v>
-      </c>
-      <c r="D69">
+        <v>1.1868238913561442</v>
+      </c>
+      <c r="C70">
         <f t="shared" si="8"/>
-        <v>0.39073112848927372</v>
-      </c>
-      <c r="E69">
+        <v>0.92718385456678742</v>
+      </c>
+      <c r="D70">
         <f t="shared" si="9"/>
-        <v>942.59696993529894</v>
-      </c>
-      <c r="F69">
-        <f t="shared" si="10"/>
-        <v>400.10867557301628</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70">
-        <f t="shared" si="11"/>
-        <v>68</v>
-      </c>
-      <c r="B70">
-        <f t="shared" si="6"/>
-        <v>1.1868238913561442</v>
-      </c>
-      <c r="C70">
+        <v>0.37460659341591196</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="10"/>
+        <v>949.43626707639032</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="10"/>
+        <v>383.59715165789385</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="11"/>
+        <v>949</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="11"/>
+        <v>384</v>
+      </c>
+      <c r="I70" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd949, 10'd384},</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A71">
+        <f t="shared" si="13"/>
+        <v>69</v>
+      </c>
+      <c r="B71">
         <f t="shared" si="7"/>
-        <v>0.92718385456678742</v>
-      </c>
-      <c r="D70">
+        <v>1.2042771838760873</v>
+      </c>
+      <c r="C71">
         <f t="shared" si="8"/>
-        <v>0.37460659341591196</v>
-      </c>
-      <c r="E70">
+        <v>0.93358042649720174</v>
+      </c>
+      <c r="D71">
         <f t="shared" si="9"/>
-        <v>949.43626707639032</v>
-      </c>
-      <c r="F70">
-        <f t="shared" si="10"/>
-        <v>383.59715165789385</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71">
-        <f t="shared" si="11"/>
-        <v>69</v>
-      </c>
-      <c r="B71">
-        <f t="shared" si="6"/>
-        <v>1.2042771838760873</v>
-      </c>
-      <c r="C71">
+        <v>0.35836794954530038</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="10"/>
+        <v>955.98635673313458</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="10"/>
+        <v>366.96878033438759</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="11"/>
+        <v>956</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="11"/>
+        <v>367</v>
+      </c>
+      <c r="I71" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd956, 10'd367},</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A72">
+        <f t="shared" si="13"/>
+        <v>70</v>
+      </c>
+      <c r="B72">
         <f t="shared" si="7"/>
-        <v>0.93358042649720174</v>
-      </c>
-      <c r="D71">
+        <v>1.2217304763960306</v>
+      </c>
+      <c r="C72">
         <f t="shared" si="8"/>
-        <v>0.35836794954530038</v>
-      </c>
-      <c r="E71">
+        <v>0.93969262078590832</v>
+      </c>
+      <c r="D72">
         <f t="shared" si="9"/>
-        <v>955.98635673313458</v>
-      </c>
-      <c r="F71">
-        <f t="shared" si="10"/>
-        <v>366.96878033438759</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72">
-        <f t="shared" si="11"/>
-        <v>70</v>
-      </c>
-      <c r="B72">
-        <f t="shared" si="6"/>
-        <v>1.2217304763960306</v>
-      </c>
-      <c r="C72">
+        <v>0.34202014332566882</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="10"/>
+        <v>962.24524368477012</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="10"/>
+        <v>350.22862676548488</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="11"/>
+        <v>962</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="11"/>
+        <v>350</v>
+      </c>
+      <c r="I72" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd962, 10'd350},</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A73">
+        <f t="shared" si="13"/>
+        <v>71</v>
+      </c>
+      <c r="B73">
         <f t="shared" si="7"/>
-        <v>0.93969262078590832</v>
-      </c>
-      <c r="D72">
+        <v>1.2391837689159739</v>
+      </c>
+      <c r="C73">
         <f t="shared" si="8"/>
-        <v>0.34202014332566882</v>
-      </c>
-      <c r="E72">
+        <v>0.94551857559931674</v>
+      </c>
+      <c r="D73">
         <f t="shared" si="9"/>
-        <v>962.24524368477012</v>
-      </c>
-      <c r="F72">
-        <f t="shared" si="10"/>
-        <v>350.22862676548488</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73">
+        <v>0.32556815445715676</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="10"/>
+        <v>968.21102141370034</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="10"/>
+        <v>333.38179016412852</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="11"/>
+        <v>968</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="11"/>
+        <v>333</v>
+      </c>
+      <c r="I73" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd968, 10'd333},</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A74">
+        <f t="shared" si="13"/>
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="7"/>
+        <v>1.2566370614359172</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="8"/>
+        <v>0.95105651629515353</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="9"/>
+        <v>0.30901699437494745</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="10"/>
+        <v>973.88187268623722</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="10"/>
+        <v>316.43340223994619</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="11"/>
+        <v>974</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="11"/>
+        <v>316</v>
+      </c>
+      <c r="I74" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd974, 10'd316},</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A75">
+        <f t="shared" si="13"/>
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="7"/>
+        <v>1.2740903539558606</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="8"/>
+        <v>0.95630475596303544</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="9"/>
+        <v>0.29237170472273677</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="10"/>
+        <v>979.25607010614829</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="10"/>
+        <v>299.38862563608245</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="11"/>
+        <v>979</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="11"/>
+        <v>299</v>
+      </c>
+      <c r="I75" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd979, 10'd299},</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A76">
+        <f t="shared" si="13"/>
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="7"/>
+        <v>1.2915436464758039</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="8"/>
+        <v>0.96126169593831889</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="9"/>
+        <v>0.27563735581699916</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="10"/>
+        <v>984.33197664083855</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="10"/>
+        <v>282.25265235660714</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="11"/>
+        <v>984</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="11"/>
+        <v>282</v>
+      </c>
+      <c r="I76" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd984, 10'd282},</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A77">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="7"/>
+        <v>1.3089969389957472</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="8"/>
+        <v>0.96592582628906831</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="9"/>
+        <v>0.25881904510252074</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="10"/>
+        <v>989.10804612000595</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="10"/>
+        <v>265.03070218498124</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="11"/>
+        <v>989</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="11"/>
+        <v>265</v>
+      </c>
+      <c r="I77" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd989, 10'd265},</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A78">
+        <f t="shared" si="13"/>
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="7"/>
+        <v>1.3264502315156905</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="8"/>
+        <v>0.97029572627599647</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="9"/>
+        <v>0.24192189559966767</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="10"/>
+        <v>993.58282370662039</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="10"/>
+        <v>247.7280210940597</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="11"/>
+        <v>994</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="11"/>
+        <v>248</v>
+      </c>
+      <c r="I78" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd994, 10'd248},</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A79">
+        <f t="shared" si="13"/>
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="7"/>
+        <v>1.3439035240356338</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="8"/>
+        <v>0.97437006478523525</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="9"/>
+        <v>0.22495105434386492</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="10"/>
+        <v>997.75494634008089</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="10"/>
+        <v>230.34987964811768</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="11"/>
+        <v>998</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="11"/>
+        <v>230</v>
+      </c>
+      <c r="I79" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd998, 10'd230},</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A80">
+        <f t="shared" si="13"/>
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="7"/>
+        <v>1.3613568165555769</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="8"/>
+        <v>0.97814760073380558</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="9"/>
+        <v>0.20791169081775945</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="10"/>
+        <v>1001.6231431514169</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="10"/>
+        <v>212.90157139738568</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="11"/>
+        <v>1002</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="11"/>
+        <v>213</v>
+      </c>
+      <c r="I80" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd1002, 10'd213},</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A81">
+        <f t="shared" si="13"/>
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="7"/>
+        <v>1.3788101090755203</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="8"/>
+        <v>0.98162718344766398</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="9"/>
+        <v>0.19080899537654492</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="10"/>
+        <v>1005.1862358504079</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="10"/>
+        <v>195.38841126558199</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="11"/>
+        <v>1005</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="11"/>
+        <v>195</v>
+      </c>
+      <c r="I81" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd1005, 10'd195},</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A82">
+        <f t="shared" si="13"/>
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="7"/>
+        <v>1.3962634015954636</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="8"/>
+        <v>0.98480775301220802</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="9"/>
+        <v>0.17364817766693041</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="10"/>
+        <v>1008.443139084501</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="10"/>
+        <v>177.81573393093674</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="11"/>
+        <v>1008</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="11"/>
+        <v>178</v>
+      </c>
+      <c r="I82" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd1008, 10'd178},</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A83">
+        <f t="shared" si="13"/>
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="7"/>
+        <v>1.4137166941154069</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="8"/>
+        <v>0.98768834059513777</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="9"/>
+        <v>0.15643446504023092</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="10"/>
+        <v>1011.3928607694211</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="10"/>
+        <v>160.18889220119647</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="11"/>
+        <v>1011</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="11"/>
+        <v>160</v>
+      </c>
+      <c r="I83" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd1011, 10'd160},</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A84">
+        <f t="shared" si="13"/>
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="7"/>
+        <v>1.4311699866353502</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="8"/>
+        <v>0.99026806874157036</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="9"/>
+        <v>0.13917310096006547</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="10"/>
+        <v>1014.0345023913681</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="10"/>
+        <v>142.51325538310704</v>
+      </c>
+      <c r="G84">
+        <f t="shared" si="11"/>
+        <v>1014</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="11"/>
+        <v>143</v>
+      </c>
+      <c r="I84" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd1014, 10'd143},</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A85">
+        <f t="shared" si="13"/>
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="7"/>
+        <v>1.4486232791552935</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="8"/>
+        <v>0.99254615164132198</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="9"/>
+        <v>0.12186934340514749</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="10"/>
+        <v>1016.3672592807137</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="10"/>
+        <v>124.79420764687103</v>
+      </c>
+      <c r="G85">
+        <f t="shared" si="11"/>
+        <v>1016</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="11"/>
+        <v>125</v>
+      </c>
+      <c r="I85" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd1016, 10'd125},</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A86">
+        <f t="shared" si="13"/>
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="7"/>
+        <v>1.4660765716752369</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="8"/>
+        <v>0.99452189536827329</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="9"/>
+        <v>0.10452846326765346</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="10"/>
+        <v>1018.3904208571118</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="10"/>
+        <v>107.03714638607714</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="11"/>
+        <v>1018</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="11"/>
+        <v>107</v>
+      </c>
+      <c r="I86" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd1018, 10'd107},</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A87">
+        <f t="shared" si="13"/>
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="7"/>
+        <v>1.4835298641951802</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="8"/>
+        <v>0.99619469809174555</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="9"/>
+        <v>8.7155742747658138E-2</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="10"/>
+        <v>1020.1033708459474</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="10"/>
+        <v>89.247480573601933</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="11"/>
+        <v>1020</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="11"/>
+        <v>89</v>
+      </c>
+      <c r="I87" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd1020, 10'd89},</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A88">
+        <f t="shared" si="13"/>
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="7"/>
+        <v>1.5009831567151235</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="8"/>
+        <v>0.9975640502598242</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="9"/>
+        <v>6.9756473744125233E-2</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="10"/>
+        <v>1021.50558746606</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="10"/>
+        <v>71.430629113984239</v>
+      </c>
+      <c r="G88">
+        <f t="shared" si="11"/>
+        <v>1022</v>
+      </c>
+      <c r="H88">
         <f t="shared" si="11"/>
         <v>71</v>
       </c>
-      <c r="B73">
-        <f t="shared" si="6"/>
-        <v>1.2391837689159739</v>
-      </c>
-      <c r="C73">
+      <c r="I88" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd1022, 10'd71},</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A89">
+        <f t="shared" si="13"/>
+        <v>87</v>
+      </c>
+      <c r="B89">
         <f t="shared" si="7"/>
-        <v>0.94551857559931674</v>
-      </c>
-      <c r="D73">
+        <v>1.5184364492350666</v>
+      </c>
+      <c r="C89">
         <f t="shared" si="8"/>
-        <v>0.32556815445715676</v>
-      </c>
-      <c r="E73">
+        <v>0.99862953475457383</v>
+      </c>
+      <c r="D89">
         <f t="shared" si="9"/>
-        <v>968.21102141370034</v>
-      </c>
-      <c r="F73">
-        <f t="shared" si="10"/>
-        <v>333.38179016412852</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74">
-        <f t="shared" si="11"/>
-        <v>72</v>
-      </c>
-      <c r="B74">
-        <f t="shared" si="6"/>
-        <v>1.2566370614359172</v>
-      </c>
-      <c r="C74">
+        <v>5.2335956242943966E-2</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="10"/>
+        <v>1022.5966435886836</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="10"/>
+        <v>53.592019192774622</v>
+      </c>
+      <c r="G89">
+        <f t="shared" si="11"/>
+        <v>1023</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="11"/>
+        <v>54</v>
+      </c>
+      <c r="I89" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd1023, 10'd54},</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A90">
+        <f t="shared" si="13"/>
+        <v>88</v>
+      </c>
+      <c r="B90">
         <f t="shared" si="7"/>
-        <v>0.95105651629515353</v>
-      </c>
-      <c r="D74">
+        <v>1.5358897417550099</v>
+      </c>
+      <c r="C90">
         <f t="shared" si="8"/>
-        <v>0.30901699437494745</v>
-      </c>
-      <c r="E74">
+        <v>0.99939082701909576</v>
+      </c>
+      <c r="D90">
         <f t="shared" si="9"/>
-        <v>973.88187268623722</v>
-      </c>
-      <c r="F74">
-        <f t="shared" si="10"/>
-        <v>316.43340223994619</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75">
-        <f t="shared" si="11"/>
-        <v>73</v>
-      </c>
-      <c r="B75">
-        <f t="shared" si="6"/>
-        <v>1.2740903539558606</v>
-      </c>
-      <c r="C75">
-        <f t="shared" si="7"/>
-        <v>0.95630475596303544</v>
-      </c>
-      <c r="D75">
-        <f t="shared" si="8"/>
-        <v>0.29237170472273677</v>
-      </c>
-      <c r="E75">
-        <f t="shared" si="9"/>
-        <v>979.25607010614829</v>
-      </c>
-      <c r="F75">
-        <f t="shared" si="10"/>
-        <v>299.38862563608245</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A76">
-        <f t="shared" si="11"/>
-        <v>74</v>
-      </c>
-      <c r="B76">
-        <f t="shared" si="6"/>
-        <v>1.2915436464758039</v>
-      </c>
-      <c r="C76">
-        <f t="shared" si="7"/>
-        <v>0.96126169593831889</v>
-      </c>
-      <c r="D76">
-        <f t="shared" si="8"/>
-        <v>0.27563735581699916</v>
-      </c>
-      <c r="E76">
-        <f t="shared" si="9"/>
-        <v>984.33197664083855</v>
-      </c>
-      <c r="F76">
-        <f t="shared" si="10"/>
-        <v>282.25265235660714</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A77">
-        <f t="shared" si="11"/>
-        <v>75</v>
-      </c>
-      <c r="B77">
-        <f t="shared" si="6"/>
-        <v>1.3089969389957472</v>
-      </c>
-      <c r="C77">
-        <f t="shared" si="7"/>
-        <v>0.96592582628906831</v>
-      </c>
-      <c r="D77">
-        <f t="shared" si="8"/>
-        <v>0.25881904510252074</v>
-      </c>
-      <c r="E77">
-        <f t="shared" si="9"/>
-        <v>989.10804612000595</v>
-      </c>
-      <c r="F77">
-        <f t="shared" si="10"/>
-        <v>265.03070218498124</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A78">
-        <f t="shared" si="11"/>
-        <v>76</v>
-      </c>
-      <c r="B78">
-        <f t="shared" si="6"/>
-        <v>1.3264502315156905</v>
-      </c>
-      <c r="C78">
-        <f t="shared" si="7"/>
-        <v>0.97029572627599647</v>
-      </c>
-      <c r="D78">
-        <f t="shared" si="8"/>
-        <v>0.24192189559966767</v>
-      </c>
-      <c r="E78">
-        <f t="shared" si="9"/>
-        <v>993.58282370662039</v>
-      </c>
-      <c r="F78">
-        <f t="shared" si="10"/>
-        <v>247.7280210940597</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A79">
-        <f t="shared" si="11"/>
-        <v>77</v>
-      </c>
-      <c r="B79">
-        <f t="shared" si="6"/>
-        <v>1.3439035240356338</v>
-      </c>
-      <c r="C79">
-        <f t="shared" si="7"/>
-        <v>0.97437006478523525</v>
-      </c>
-      <c r="D79">
-        <f t="shared" si="8"/>
-        <v>0.22495105434386492</v>
-      </c>
-      <c r="E79">
-        <f t="shared" si="9"/>
-        <v>997.75494634008089</v>
-      </c>
-      <c r="F79">
-        <f t="shared" si="10"/>
-        <v>230.34987964811768</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A80">
-        <f t="shared" si="11"/>
-        <v>78</v>
-      </c>
-      <c r="B80">
-        <f t="shared" si="6"/>
-        <v>1.3613568165555769</v>
-      </c>
-      <c r="C80">
-        <f t="shared" si="7"/>
-        <v>0.97814760073380558</v>
-      </c>
-      <c r="D80">
-        <f t="shared" si="8"/>
-        <v>0.20791169081775945</v>
-      </c>
-      <c r="E80">
-        <f t="shared" si="9"/>
-        <v>1001.6231431514169</v>
-      </c>
-      <c r="F80">
-        <f t="shared" si="10"/>
-        <v>212.90157139738568</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A81">
-        <f t="shared" si="11"/>
-        <v>79</v>
-      </c>
-      <c r="B81">
-        <f t="shared" si="6"/>
-        <v>1.3788101090755203</v>
-      </c>
-      <c r="C81">
-        <f t="shared" si="7"/>
-        <v>0.98162718344766398</v>
-      </c>
-      <c r="D81">
-        <f t="shared" si="8"/>
-        <v>0.19080899537654492</v>
-      </c>
-      <c r="E81">
-        <f t="shared" si="9"/>
-        <v>1005.1862358504079</v>
-      </c>
-      <c r="F81">
-        <f t="shared" si="10"/>
-        <v>195.38841126558199</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A82">
-        <f t="shared" si="11"/>
-        <v>80</v>
-      </c>
-      <c r="B82">
-        <f t="shared" si="6"/>
-        <v>1.3962634015954636</v>
-      </c>
-      <c r="C82">
-        <f t="shared" si="7"/>
-        <v>0.98480775301220802</v>
-      </c>
-      <c r="D82">
-        <f t="shared" si="8"/>
-        <v>0.17364817766693041</v>
-      </c>
-      <c r="E82">
-        <f t="shared" si="9"/>
-        <v>1008.443139084501</v>
-      </c>
-      <c r="F82">
-        <f t="shared" si="10"/>
-        <v>177.81573393093674</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A83">
-        <f t="shared" si="11"/>
-        <v>81</v>
-      </c>
-      <c r="B83">
-        <f t="shared" si="6"/>
-        <v>1.4137166941154069</v>
-      </c>
-      <c r="C83">
-        <f t="shared" si="7"/>
-        <v>0.98768834059513777</v>
-      </c>
-      <c r="D83">
-        <f t="shared" si="8"/>
-        <v>0.15643446504023092</v>
-      </c>
-      <c r="E83">
-        <f t="shared" si="9"/>
-        <v>1011.3928607694211</v>
-      </c>
-      <c r="F83">
-        <f t="shared" si="10"/>
-        <v>160.18889220119647</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A84">
-        <f t="shared" si="11"/>
-        <v>82</v>
-      </c>
-      <c r="B84">
-        <f t="shared" si="6"/>
-        <v>1.4311699866353502</v>
-      </c>
-      <c r="C84">
-        <f t="shared" si="7"/>
-        <v>0.99026806874157036</v>
-      </c>
-      <c r="D84">
-        <f t="shared" si="8"/>
-        <v>0.13917310096006547</v>
-      </c>
-      <c r="E84">
-        <f t="shared" si="9"/>
-        <v>1014.0345023913681</v>
-      </c>
-      <c r="F84">
-        <f t="shared" si="10"/>
-        <v>142.51325538310704</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A85">
-        <f t="shared" si="11"/>
-        <v>83</v>
-      </c>
-      <c r="B85">
-        <f t="shared" si="6"/>
-        <v>1.4486232791552935</v>
-      </c>
-      <c r="C85">
-        <f t="shared" si="7"/>
-        <v>0.99254615164132198</v>
-      </c>
-      <c r="D85">
-        <f t="shared" si="8"/>
-        <v>0.12186934340514749</v>
-      </c>
-      <c r="E85">
-        <f t="shared" si="9"/>
-        <v>1016.3672592807137</v>
-      </c>
-      <c r="F85">
-        <f t="shared" si="10"/>
-        <v>124.79420764687103</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A86">
-        <f t="shared" si="11"/>
-        <v>84</v>
-      </c>
-      <c r="B86">
-        <f t="shared" si="6"/>
-        <v>1.4660765716752369</v>
-      </c>
-      <c r="C86">
-        <f t="shared" si="7"/>
-        <v>0.99452189536827329</v>
-      </c>
-      <c r="D86">
-        <f t="shared" si="8"/>
-        <v>0.10452846326765346</v>
-      </c>
-      <c r="E86">
-        <f t="shared" si="9"/>
-        <v>1018.3904208571118</v>
-      </c>
-      <c r="F86">
-        <f t="shared" si="10"/>
-        <v>107.03714638607714</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A87">
-        <f t="shared" si="11"/>
-        <v>85</v>
-      </c>
-      <c r="B87">
-        <f t="shared" si="6"/>
-        <v>1.4835298641951802</v>
-      </c>
-      <c r="C87">
-        <f t="shared" si="7"/>
-        <v>0.99619469809174555</v>
-      </c>
-      <c r="D87">
-        <f t="shared" si="8"/>
-        <v>8.7155742747658138E-2</v>
-      </c>
-      <c r="E87">
-        <f t="shared" si="9"/>
-        <v>1020.1033708459474</v>
-      </c>
-      <c r="F87">
-        <f t="shared" si="10"/>
-        <v>89.247480573601933</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A88">
-        <f t="shared" si="11"/>
-        <v>86</v>
-      </c>
-      <c r="B88">
-        <f t="shared" si="6"/>
-        <v>1.5009831567151235</v>
-      </c>
-      <c r="C88">
-        <f t="shared" si="7"/>
-        <v>0.9975640502598242</v>
-      </c>
-      <c r="D88">
-        <f t="shared" si="8"/>
-        <v>6.9756473744125233E-2</v>
-      </c>
-      <c r="E88">
-        <f t="shared" si="9"/>
-        <v>1021.50558746606</v>
-      </c>
-      <c r="F88">
-        <f t="shared" si="10"/>
-        <v>71.430629113984239</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A89">
-        <f t="shared" si="11"/>
-        <v>87</v>
-      </c>
-      <c r="B89">
-        <f t="shared" si="6"/>
-        <v>1.5184364492350666</v>
-      </c>
-      <c r="C89">
-        <f t="shared" si="7"/>
-        <v>0.99862953475457383</v>
-      </c>
-      <c r="D89">
-        <f t="shared" si="8"/>
-        <v>5.2335956242943966E-2</v>
-      </c>
-      <c r="E89">
-        <f t="shared" si="9"/>
-        <v>1022.5966435886836</v>
-      </c>
-      <c r="F89">
-        <f t="shared" si="10"/>
-        <v>53.592019192774622</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A90">
-        <f t="shared" si="11"/>
-        <v>88</v>
-      </c>
-      <c r="B90">
-        <f t="shared" si="6"/>
-        <v>1.5358897417550099</v>
-      </c>
-      <c r="C90">
-        <f t="shared" si="7"/>
-        <v>0.99939082701909576</v>
-      </c>
-      <c r="D90">
-        <f t="shared" si="8"/>
         <v>3.489949670250108E-2</v>
       </c>
       <c r="E90">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1023.3762068675541</v>
       </c>
       <c r="F90">
         <f t="shared" si="10"/>
         <v>35.737084623361106</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G90">
+        <f t="shared" si="11"/>
+        <v>1023</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="11"/>
+        <v>36</v>
+      </c>
+      <c r="I90" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd1023, 10'd36},</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91">
         <f xml:space="preserve"> A90 + 1</f>
         <v>89</v>
       </c>
       <c r="B91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.5533430342749532</v>
       </c>
       <c r="C91">
+        <f t="shared" si="8"/>
+        <v>0.99984769515639127</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="9"/>
+        <v>1.7452406437283598E-2</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="10"/>
+        <v>1023.8440398401447</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="10"/>
+        <v>17.871264191778405</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="11"/>
+        <v>1024</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="11"/>
+        <v>18</v>
+      </c>
+      <c r="I91" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd1024, 10'd18},</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A92">
+        <f t="shared" ref="A92" si="14" xml:space="preserve"> A91 + 1</f>
+        <v>90</v>
+      </c>
+      <c r="B92">
         <f t="shared" si="7"/>
-        <v>0.99984769515639127</v>
-      </c>
-      <c r="D91">
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="C92">
         <f t="shared" si="8"/>
-        <v>1.7452406437283598E-2</v>
-      </c>
-      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="D92">
         <f t="shared" si="9"/>
-        <v>1023.8440398401447</v>
-      </c>
-      <c r="F91">
-        <f t="shared" si="10"/>
-        <v>17.871264191778405</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A92">
-        <f t="shared" ref="A92" si="12" xml:space="preserve"> A91 + 1</f>
-        <v>90</v>
-      </c>
-      <c r="B92">
-        <f t="shared" si="6"/>
-        <v>1.5707963267948966</v>
-      </c>
-      <c r="C92">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="D92">
-        <f t="shared" si="8"/>
         <v>6.1257422745431001E-17</v>
       </c>
       <c r="E92">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1024</v>
       </c>
       <c r="F92">
         <f t="shared" si="10"/>
         <v>6.2727600891321345E-14</v>
+      </c>
+      <c r="G92">
+        <f t="shared" si="11"/>
+        <v>1024</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="I92" t="str">
+        <f t="shared" si="12"/>
+        <v>{10'd1024, 10'd0},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>